<commit_message>
Takım isim eşleşmesi düzeltildi (FC St. Pauli sorunu fix)
</commit_message>
<xml_diff>
--- a/data/bundesliga_matches_2023_2025.xlsx
+++ b/data/bundesliga_matches_2023_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J630"/>
+  <dimension ref="A1:J639"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25645,6 +25645,366 @@
         </is>
       </c>
     </row>
+    <row r="631">
+      <c r="A631" t="n">
+        <v>540425</v>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>2025-09-12T18:30:00Z</t>
+        </is>
+      </c>
+      <c r="C631" t="n">
+        <v>3</v>
+      </c>
+      <c r="D631" t="n">
+        <v>3</v>
+      </c>
+      <c r="E631" t="inlineStr">
+        <is>
+          <t>Bayer 04 Leverkusen</t>
+        </is>
+      </c>
+      <c r="F631" t="n">
+        <v>19</v>
+      </c>
+      <c r="G631" t="inlineStr">
+        <is>
+          <t>Eintracht Frankfurt</t>
+        </is>
+      </c>
+      <c r="H631" t="n">
+        <v>3</v>
+      </c>
+      <c r="I631" t="n">
+        <v>1</v>
+      </c>
+      <c r="J631" t="inlineStr">
+        <is>
+          <t>HomeWin</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="n">
+        <v>540426</v>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:30:00Z</t>
+        </is>
+      </c>
+      <c r="C632" t="n">
+        <v>3</v>
+      </c>
+      <c r="D632" t="n">
+        <v>17</v>
+      </c>
+      <c r="E632" t="inlineStr">
+        <is>
+          <t>SC Freiburg</t>
+        </is>
+      </c>
+      <c r="F632" t="n">
+        <v>10</v>
+      </c>
+      <c r="G632" t="inlineStr">
+        <is>
+          <t>VfB Stuttgart</t>
+        </is>
+      </c>
+      <c r="H632" t="n">
+        <v>3</v>
+      </c>
+      <c r="I632" t="n">
+        <v>1</v>
+      </c>
+      <c r="J632" t="inlineStr">
+        <is>
+          <t>HomeWin</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="n">
+        <v>540427</v>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:30:00Z</t>
+        </is>
+      </c>
+      <c r="C633" t="n">
+        <v>3</v>
+      </c>
+      <c r="D633" t="n">
+        <v>15</v>
+      </c>
+      <c r="E633" t="inlineStr">
+        <is>
+          <t>1. FSV Mainz 05</t>
+        </is>
+      </c>
+      <c r="F633" t="n">
+        <v>721</v>
+      </c>
+      <c r="G633" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="H633" t="n">
+        <v>0</v>
+      </c>
+      <c r="I633" t="n">
+        <v>1</v>
+      </c>
+      <c r="J633" t="inlineStr">
+        <is>
+          <t>AwayWin</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="n">
+        <v>540429</v>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:30:00Z</t>
+        </is>
+      </c>
+      <c r="C634" t="n">
+        <v>3</v>
+      </c>
+      <c r="D634" t="n">
+        <v>11</v>
+      </c>
+      <c r="E634" t="inlineStr">
+        <is>
+          <t>VfL Wolfsburg</t>
+        </is>
+      </c>
+      <c r="F634" t="n">
+        <v>1</v>
+      </c>
+      <c r="G634" t="inlineStr">
+        <is>
+          <t>1. FC Köln</t>
+        </is>
+      </c>
+      <c r="H634" t="n">
+        <v>3</v>
+      </c>
+      <c r="I634" t="n">
+        <v>3</v>
+      </c>
+      <c r="J634" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="n">
+        <v>540430</v>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:30:00Z</t>
+        </is>
+      </c>
+      <c r="C635" t="n">
+        <v>3</v>
+      </c>
+      <c r="D635" t="n">
+        <v>28</v>
+      </c>
+      <c r="E635" t="inlineStr">
+        <is>
+          <t>1. FC Union Berlin</t>
+        </is>
+      </c>
+      <c r="F635" t="n">
+        <v>2</v>
+      </c>
+      <c r="G635" t="inlineStr">
+        <is>
+          <t>TSG 1899 Hoffenheim</t>
+        </is>
+      </c>
+      <c r="H635" t="n">
+        <v>2</v>
+      </c>
+      <c r="I635" t="n">
+        <v>4</v>
+      </c>
+      <c r="J635" t="inlineStr">
+        <is>
+          <t>AwayWin</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="n">
+        <v>540432</v>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:30:00Z</t>
+        </is>
+      </c>
+      <c r="C636" t="n">
+        <v>3</v>
+      </c>
+      <c r="D636" t="n">
+        <v>44</v>
+      </c>
+      <c r="E636" t="inlineStr">
+        <is>
+          <t>1. FC Heidenheim 1846</t>
+        </is>
+      </c>
+      <c r="F636" t="n">
+        <v>4</v>
+      </c>
+      <c r="G636" t="inlineStr">
+        <is>
+          <t>Borussia Dortmund</t>
+        </is>
+      </c>
+      <c r="H636" t="n">
+        <v>0</v>
+      </c>
+      <c r="I636" t="n">
+        <v>2</v>
+      </c>
+      <c r="J636" t="inlineStr">
+        <is>
+          <t>AwayWin</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="n">
+        <v>540424</v>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>2025-09-13T16:30:00Z</t>
+        </is>
+      </c>
+      <c r="C637" t="n">
+        <v>3</v>
+      </c>
+      <c r="D637" t="n">
+        <v>5</v>
+      </c>
+      <c r="E637" t="inlineStr">
+        <is>
+          <t>FC Bayern München</t>
+        </is>
+      </c>
+      <c r="F637" t="n">
+        <v>7</v>
+      </c>
+      <c r="G637" t="inlineStr">
+        <is>
+          <t>Hamburger SV</t>
+        </is>
+      </c>
+      <c r="H637" t="n">
+        <v>5</v>
+      </c>
+      <c r="I637" t="n">
+        <v>0</v>
+      </c>
+      <c r="J637" t="inlineStr">
+        <is>
+          <t>HomeWin</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="n">
+        <v>540431</v>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>2025-09-14T13:30:00Z</t>
+        </is>
+      </c>
+      <c r="C638" t="n">
+        <v>3</v>
+      </c>
+      <c r="D638" t="n">
+        <v>20</v>
+      </c>
+      <c r="E638" t="inlineStr">
+        <is>
+          <t>FC St. Pauli 1910</t>
+        </is>
+      </c>
+      <c r="F638" t="n">
+        <v>16</v>
+      </c>
+      <c r="G638" t="inlineStr">
+        <is>
+          <t>FC Augsburg</t>
+        </is>
+      </c>
+      <c r="H638" t="n">
+        <v>2</v>
+      </c>
+      <c r="I638" t="n">
+        <v>1</v>
+      </c>
+      <c r="J638" t="inlineStr">
+        <is>
+          <t>HomeWin</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="n">
+        <v>540428</v>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>2025-09-14T15:30:00Z</t>
+        </is>
+      </c>
+      <c r="C639" t="n">
+        <v>3</v>
+      </c>
+      <c r="D639" t="n">
+        <v>18</v>
+      </c>
+      <c r="E639" t="inlineStr">
+        <is>
+          <t>Borussia Mönchengladbach</t>
+        </is>
+      </c>
+      <c r="F639" t="n">
+        <v>12</v>
+      </c>
+      <c r="G639" t="inlineStr">
+        <is>
+          <t>SV Werder Bremen</t>
+        </is>
+      </c>
+      <c r="H639" t="n">
+        <v>0</v>
+      </c>
+      <c r="I639" t="n">
+        <v>4</v>
+      </c>
+      <c r="J639" t="inlineStr">
+        <is>
+          <t>AwayWin</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>